<commit_message>
GCP- svm & ANN finished
</commit_message>
<xml_diff>
--- a/feature_selection/Univariante ROC_AUC/Qualitative deleted/Continuous deleted/Balancing_Oversamlping_SMOTE/tables_smote.xlsx
+++ b/feature_selection/Univariante ROC_AUC/Qualitative deleted/Continuous deleted/Balancing_Oversamlping_SMOTE/tables_smote.xlsx
@@ -13,6 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="XGB_smote1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="XGB_smote2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="XGB_smote3" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SVM_Z" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SVM_Z1" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4610,4 +4612,641 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Precision(Avg)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Recall(Avg)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 1]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.8202016936184913</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8398572549632499</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.820282038885024</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.1]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8313459531047886</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.851020859901092</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.8314250498125393</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.01]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8331429606852417</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8523256289622969</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8332208987570006</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.001]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.7531690989279278</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7804823936473813</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.7532732474442394</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.834118037522918</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8445046745608472</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8341759138897922</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.1]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8337558885243981</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8520001665666375</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8338319426194308</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.01]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8330315080582551</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8517541222750274</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8331085777033153</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.001]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.833741960948202</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8522439273924404</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8338185079466743</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>[10, 1]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8262892474949499</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8302048856613891</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8263254969347413</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.1]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8352046261712905</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8490241558064276</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8352709256667555</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.01]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8337698180410438</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8522249218111486</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8338462777238455</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.001]</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8329061356168698</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8515586436603563</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.8329830800585452</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>[100, 1]</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.8121639162104985</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8133813418809875</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.8121842487838122</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.1]</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8362493826096122</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8471648237403262</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.8363086445043949</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.01]</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.8339230495157206</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.852221501104734</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8339991861698973</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.001]</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.8336026541390471</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8520668801586948</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8336791583789573</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Precision(Avg)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Recall(Avg)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>std_cross_validation</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 1]</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.8202016936184913</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.8398572549632499</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.820282038885024</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.002454186493353154</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.1]</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8313459531047886</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.851020859901092</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.8314250498125393</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.002019755326894574</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.01]</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.8331429606852417</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8523256289622969</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8332208987570006</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002249333580720828</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>[0.1, 0.001]</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.7531690989279278</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7804823936473813</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.7532732474442394</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.003187951894907381</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>[1, 1]</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.834118037522918</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8445046745608472</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8341759138897922</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.003089174059208984</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.1]</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8337558885243981</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8520001665666375</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.8338319426194308</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002057226086398187</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.01]</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8330315080582551</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8517541222750274</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8331085777033153</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.00202820335174945</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>[1, 0.001]</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.833741960948202</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8522439273924404</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8338185079466743</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.002345544505908686</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>[10, 1]</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.8262892474949499</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.8302048856613891</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.8263254969347413</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.002092907043063291</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.1]</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.8352046261712905</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8490241558064276</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8352709256667555</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.002501541426657304</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.01]</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.8337698180410438</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8522249218111486</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8338462777238455</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.002076162180536619</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>[10, 0.001]</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8329061356168698</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8515586436603563</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.8329830800585452</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.002295507980122763</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>[100, 1]</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.8121639162104985</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8133813418809875</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.8121842487838122</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0009202182752484279</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.1]</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.8362493826096122</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8471648237403262</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.8363086445043949</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.003235119973930643</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.01]</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.8339230495157206</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.852221501104734</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8339991861698973</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.002037621877036707</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>[100, 0.001]</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.8336026541390471</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8520668801586948</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8336791583789573</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.00213853529598701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>